<commit_message>
3rd Commit - React Config
</commit_message>
<xml_diff>
--- a/public/resources/contenido.xlsx
+++ b/public/resources/contenido.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcima/Skylab/skylab-partTimeFront-201805/staff/ariel/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcima/Skylab/jammint/public/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3FC61D-9961-794A-B536-DB66D0C3E674}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F671AA-970A-874B-8EEA-BD49A7B47974}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26740" windowHeight="14420" activeTab="1" xr2:uid="{C3C59CB8-E142-534B-B54B-2F07D83096D0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="130">
   <si>
     <t>Registro usuario</t>
   </si>
@@ -413,13 +413,19 @@
     <t xml:space="preserve">  {User ID, Text, img, date, time}</t>
   </si>
   <si>
-    <t>Lat Board Visit</t>
-  </si>
-  <si>
     <t xml:space="preserve">   {date}</t>
   </si>
   <si>
     <t>Picture: String</t>
+  </si>
+  <si>
+    <t>Jam acceptance: boolean</t>
+  </si>
+  <si>
+    <t>Comments: String</t>
+  </si>
+  <si>
+    <t>Last Board Visit</t>
   </si>
 </sst>
 </file>
@@ -525,7 +531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -548,6 +554,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -557,14 +570,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -999,16 +1004,16 @@
   <dimension ref="C3:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="4.1640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.1640625" style="12" customWidth="1"/>
     <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.1640625" customWidth="1"/>
     <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
@@ -1017,21 +1022,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="10" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1142,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="E10" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G10" t="s">
         <v>97</v>
@@ -1159,7 +1164,7 @@
         <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G11" t="s">
         <v>99</v>
@@ -1169,13 +1174,19 @@
       <c r="C12" t="s">
         <v>90</v>
       </c>
+      <c r="E12" t="s">
+        <v>127</v>
+      </c>
       <c r="G12" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="E13" t="s">
+        <v>128</v>
       </c>
       <c r="G13" t="s">
         <v>104</v>
@@ -1275,7 +1286,7 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1283,19 +1294,19 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="10"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="10"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1303,19 +1314,19 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="10"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="10"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1323,13 +1334,13 @@
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="10"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1337,13 +1348,13 @@
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="10"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1351,7 +1362,7 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="12"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Register & Login components
</commit_message>
<xml_diff>
--- a/public/resources/contenido.xlsx
+++ b/public/resources/contenido.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcima/Skylab/jammint/public/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F671AA-970A-874B-8EEA-BD49A7B47974}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8607F919-2003-5045-A797-52ED57FD9DD7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26740" windowHeight="14420" activeTab="1" xr2:uid="{C3C59CB8-E142-534B-B54B-2F07D83096D0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="132">
   <si>
     <t>Registro usuario</t>
   </si>
@@ -426,6 +426,12 @@
   </si>
   <si>
     <t>Last Board Visit</t>
+  </si>
+  <si>
+    <t>Agency: String</t>
+  </si>
+  <si>
+    <t>Agency Commision: Nr</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1010,7 @@
   <dimension ref="C3:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1193,11 +1199,17 @@
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>130</v>
+      </c>
       <c r="G14" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>131</v>
+      </c>
       <c r="G15" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
Bugs fixing and css-ing
</commit_message>
<xml_diff>
--- a/public/resources/contenido.xlsx
+++ b/public/resources/contenido.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcima/Skylab/jammint/public/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8607F919-2003-5045-A797-52ED57FD9DD7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25DE2A2-5C21-6945-BBBC-B33BD4166DC5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26740" windowHeight="14420" activeTab="1" xr2:uid="{C3C59CB8-E142-534B-B54B-2F07D83096D0}"/>
+    <workbookView xWindow="8560" yWindow="640" windowWidth="28940" windowHeight="14420" activeTab="1" xr2:uid="{C3C59CB8-E142-534B-B54B-2F07D83096D0}"/>
   </bookViews>
   <sheets>
     <sheet name="PROCESS" sheetId="4" r:id="rId1"/>
     <sheet name="DATA" sheetId="10" r:id="rId2"/>
-    <sheet name="MAIN" sheetId="9" r:id="rId3"/>
-    <sheet name="GRAL" sheetId="3" r:id="rId4"/>
-    <sheet name="BOARD" sheetId="1" r:id="rId5"/>
-    <sheet name="J'ers" sheetId="2" r:id="rId6"/>
-    <sheet name="PRIV AREA" sheetId="7" r:id="rId7"/>
-    <sheet name="CREATE" sheetId="5" r:id="rId8"/>
-    <sheet name="SIGNIN" sheetId="6" r:id="rId9"/>
+    <sheet name="Technologies" sheetId="11" r:id="rId3"/>
+    <sheet name="MAIN" sheetId="9" r:id="rId4"/>
+    <sheet name="GRAL" sheetId="3" r:id="rId5"/>
+    <sheet name="BOARD" sheetId="1" r:id="rId6"/>
+    <sheet name="J'ers" sheetId="2" r:id="rId7"/>
+    <sheet name="PRIV AREA" sheetId="7" r:id="rId8"/>
+    <sheet name="CREATE" sheetId="5" r:id="rId9"/>
+    <sheet name="SIGNIN" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="142">
   <si>
     <t>Registro usuario</t>
   </si>
@@ -432,6 +433,36 @@
   </si>
   <si>
     <t>Agency Commision: Nr</t>
+  </si>
+  <si>
+    <t>Transversal</t>
+  </si>
+  <si>
+    <t>Server-Side</t>
+  </si>
+  <si>
+    <t>Client-side</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Agile Methodology</t>
+  </si>
+  <si>
+    <t>Javascript</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>Firebase</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>CSS3 /Sass</t>
   </si>
 </sst>
 </file>
@@ -483,7 +514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -532,12 +563,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -560,13 +602,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -575,6 +617,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1005,222 +1055,339 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE57317-038A-764A-9820-2888368BDB04}">
+  <dimension ref="C3:M86"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C82" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G82" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>38</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>39</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>40</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>41</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81120CBC-F352-FC44-A471-682828A3D98D}">
   <dimension ref="C3:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" style="11" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.1640625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="4.1640625" style="11" customWidth="1"/>
     <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.1640625" customWidth="1"/>
-    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.1640625" customWidth="1"/>
     <col min="10" max="10" width="4.1640625" customWidth="1"/>
     <col min="11" max="11" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="19" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
+      <c r="C4" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="17" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
+      <c r="C5" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="17" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
+      <c r="C6" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="17" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
+      <c r="C7" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="17" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+      <c r="C8" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="17" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
+      <c r="C9" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="17" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
+      <c r="C10" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="18" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
+      <c r="C11" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="17" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+      <c r="C12" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="17" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
+      <c r="C13" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="E14" t="s">
+      <c r="E14" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="17" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="E15" t="s">
+      <c r="E15" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G16" t="s">
+      <c r="G16" s="17" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G17" t="s">
+      <c r="G17" s="18" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1230,6 +1397,69 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB2C386-EC15-6C4C-BAD3-CAB463BBAACE}">
+  <dimension ref="B5:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="5" width="18.33203125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF18D40-6E20-AE47-9220-46669BAF7859}">
   <dimension ref="C2:G8"/>
   <sheetViews>
@@ -1282,7 +1512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A1CA7D2-85C9-0544-8551-3CE116867EE0}">
   <dimension ref="B4:C15"/>
   <sheetViews>
@@ -1391,7 +1621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3594728-C2B3-7E46-BDE6-81EFAB90C096}">
   <dimension ref="C4:G8"/>
   <sheetViews>
@@ -1461,7 +1691,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5D6A1D-B023-2147-AD40-EE80969E5930}">
   <dimension ref="C3:M19"/>
   <sheetViews>
@@ -1554,7 +1784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B700D30D-4EE5-3643-815E-8F443882E2B2}">
   <dimension ref="C3:M13"/>
   <sheetViews>
@@ -1667,7 +1897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841FB19C-6CE2-9545-81C4-F0C3FF67A91B}">
   <dimension ref="C3:M86"/>
   <sheetViews>
@@ -1830,121 +2060,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE57317-038A-764A-9820-2888368BDB04}">
-  <dimension ref="C3:M86"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="10.83203125" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C82" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F82" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G82" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C83" t="s">
-        <v>38</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C84" t="s">
-        <v>39</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C85" t="s">
-        <v>40</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C86" t="s">
-        <v>41</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>